<commit_message>
fix typo of unnecessary spaces at the end of interest group
</commit_message>
<xml_diff>
--- a/Interest-group-09-25.xlsx
+++ b/Interest-group-09-25.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Dropbox/2017 Fall/amicus brief/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Documents/Amicus-Brief/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="2040" windowWidth="19740" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="19740" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Interest-group-09-15" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="204">
   <si>
     <t>CASE-NAME</t>
   </si>
@@ -377,15 +377,9 @@
     <t>LATINO-ASIAN-2</t>
   </si>
   <si>
-    <t xml:space="preserve">NATIONAL COALITION FOR HAITIAN RIGHTS </t>
-  </si>
-  <si>
     <t>ORGANIZATION OF CHINESE AMERICANS</t>
   </si>
   <si>
-    <t xml:space="preserve">CAMBODIAN ASSOCIATION OF AMERICA </t>
-  </si>
-  <si>
     <t>HMONG NATIONAL DEVELOPMENT</t>
   </si>
   <si>
@@ -419,24 +413,9 @@
     <t>LATINO-2</t>
   </si>
   <si>
-    <t xml:space="preserve">ARIZONA HISPANIC CHAMBER OF COMMERCE </t>
-  </si>
-  <si>
     <t xml:space="preserve">MEXICAN AMERICAN LEGAL DEFENSE AND EDUCATIONAL FUND </t>
   </si>
   <si>
-    <t xml:space="preserve">ASIAN AMERICAN JUSTICE CENTER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASIAN PACIFIC AMERICAN LEGAL CENTER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASIAN CHAMBER OF COMMERCE OF ARIZONA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAPANESE AMERICAN CITIZENS LEAGUE </t>
-  </si>
-  <si>
     <t>CRAWFORD V. LA BOARD OF EDUCATION</t>
   </si>
   <si>
@@ -470,9 +449,6 @@
     <t>87-998</t>
   </si>
   <si>
-    <t xml:space="preserve">MARYLAND LEGISLATIVE BLACK CAUCUS </t>
-  </si>
-  <si>
     <t>COUNCIL OF ASIAN-AMERICAN BUSINESS ASSOCIATION</t>
   </si>
   <si>
@@ -488,21 +464,12 @@
     <t>CONGRESSIONAL BLACK CAUCUS</t>
   </si>
   <si>
-    <t xml:space="preserve">NATIONAL BLACK MEDIA COALITION </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEAGUE OF UNITED LATIN AMERICAN CITIZENS </t>
-  </si>
-  <si>
     <t>ROMER V. EVANS</t>
   </si>
   <si>
     <t>94-1039</t>
   </si>
   <si>
-    <t xml:space="preserve">ASIAN AMERICAN LEGAL DEFENSE AND EDUCATION FUND </t>
-  </si>
-  <si>
     <t>CITY OF CHICAGO V. MORALES</t>
   </si>
   <si>
@@ -648,6 +615,27 @@
   </si>
   <si>
     <t>INTEREST-GROUP</t>
+  </si>
+  <si>
+    <t>MEXICAN AMERICAN LEGAL DEFENSE AND EDUCATIONAL FUND</t>
+  </si>
+  <si>
+    <t>NATIONAL COALITION FOR HAITIAN RIGHTS</t>
+  </si>
+  <si>
+    <t>CAMBODIAN ASSOCIATION OF AMERICA</t>
+  </si>
+  <si>
+    <t>ARIZONA HISPANIC CHAMBER OF COMMERCE</t>
+  </si>
+  <si>
+    <t>ASIAN CHAMBER OF COMMERCE OF ARIZONA</t>
+  </si>
+  <si>
+    <t>MARYLAND LEGISLATIVE BLACK CAUCUS</t>
+  </si>
+  <si>
+    <t>NATIONAL BLACK MEDIA COALITION</t>
   </si>
 </sst>
 </file>
@@ -965,14 +953,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="F261" sqref="F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -992,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1032,7 +1021,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1152,7 +1141,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1372,7 +1361,7 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1532,7 +1521,7 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>117</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1572,7 +1561,7 @@
         <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1592,7 +1581,7 @@
         <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1612,7 +1601,7 @@
         <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1872,7 +1861,7 @@
         <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1952,7 +1941,7 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1977,10 +1966,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C51">
         <v>2012</v>
@@ -1997,10 +1986,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C52">
         <v>2012</v>
@@ -2012,15 +2001,15 @@
         <v>15</v>
       </c>
       <c r="F52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C53">
         <v>2012</v>
@@ -2032,15 +2021,15 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C54">
         <v>2012</v>
@@ -2057,10 +2046,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C55">
         <v>2012</v>
@@ -2077,10 +2066,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C56">
         <v>2012</v>
@@ -2092,15 +2081,15 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C57">
         <v>2012</v>
@@ -2117,10 +2106,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C58">
         <v>2012</v>
@@ -2132,15 +2121,15 @@
         <v>15</v>
       </c>
       <c r="F58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C59">
         <v>2012</v>
@@ -2152,15 +2141,15 @@
         <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C60">
         <v>2012</v>
@@ -2172,15 +2161,15 @@
         <v>8</v>
       </c>
       <c r="F60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C61">
         <v>2012</v>
@@ -2192,15 +2181,15 @@
         <v>14</v>
       </c>
       <c r="F61" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C62">
         <v>2012</v>
@@ -2217,10 +2206,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C63">
         <v>2012</v>
@@ -2237,10 +2226,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C64">
         <v>2012</v>
@@ -2257,10 +2246,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C65">
         <v>2012</v>
@@ -2277,10 +2266,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C66">
         <v>2012</v>
@@ -2297,10 +2286,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C67">
         <v>2012</v>
@@ -2317,30 +2306,30 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C68">
         <v>2012</v>
       </c>
       <c r="D68" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E68" t="s">
         <v>14</v>
       </c>
       <c r="F68" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C69">
         <v>2012</v>
@@ -2352,15 +2341,15 @@
         <v>14</v>
       </c>
       <c r="F69" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C70">
         <v>2012</v>
@@ -2372,15 +2361,15 @@
         <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C71">
         <v>2012</v>
@@ -2392,15 +2381,15 @@
         <v>8</v>
       </c>
       <c r="F71" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C72">
         <v>2012</v>
@@ -2412,15 +2401,15 @@
         <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73">
         <v>2012</v>
@@ -2432,7 +2421,7 @@
         <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2752,7 +2741,7 @@
         <v>14</v>
       </c>
       <c r="F89" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2892,7 +2881,7 @@
         <v>14</v>
       </c>
       <c r="F96" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -3080,7 +3069,7 @@
         <v>78</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C106">
         <v>2013</v>
@@ -3100,7 +3089,7 @@
         <v>78</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C107">
         <v>2013</v>
@@ -3120,7 +3109,7 @@
         <v>78</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C108">
         <v>2013</v>
@@ -3140,7 +3129,7 @@
         <v>78</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C109">
         <v>2013</v>
@@ -3160,7 +3149,7 @@
         <v>78</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C110">
         <v>2013</v>
@@ -3180,7 +3169,7 @@
         <v>78</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C111">
         <v>2013</v>
@@ -3200,7 +3189,7 @@
         <v>78</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C112">
         <v>2013</v>
@@ -3220,7 +3209,7 @@
         <v>78</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C113">
         <v>2013</v>
@@ -3240,7 +3229,7 @@
         <v>78</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C114">
         <v>2013</v>
@@ -3260,7 +3249,7 @@
         <v>78</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C115">
         <v>2013</v>
@@ -3280,7 +3269,7 @@
         <v>78</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C116">
         <v>2013</v>
@@ -3300,7 +3289,7 @@
         <v>78</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C117">
         <v>2013</v>
@@ -3320,7 +3309,7 @@
         <v>78</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C118">
         <v>2013</v>
@@ -3340,7 +3329,7 @@
         <v>78</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C119">
         <v>2013</v>
@@ -3360,7 +3349,7 @@
         <v>78</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C120">
         <v>2013</v>
@@ -3380,7 +3369,7 @@
         <v>78</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C121">
         <v>2013</v>
@@ -3400,7 +3389,7 @@
         <v>78</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C122">
         <v>2013</v>
@@ -3420,7 +3409,7 @@
         <v>78</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C123">
         <v>2013</v>
@@ -3440,7 +3429,7 @@
         <v>78</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C124">
         <v>2013</v>
@@ -3460,7 +3449,7 @@
         <v>78</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C125">
         <v>2013</v>
@@ -3480,7 +3469,7 @@
         <v>78</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C126">
         <v>2013</v>
@@ -3500,7 +3489,7 @@
         <v>78</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C127">
         <v>2013</v>
@@ -3520,7 +3509,7 @@
         <v>78</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C128">
         <v>2013</v>
@@ -3540,7 +3529,7 @@
         <v>78</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C129">
         <v>2013</v>
@@ -3560,7 +3549,7 @@
         <v>78</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C130">
         <v>2013</v>
@@ -3580,7 +3569,7 @@
         <v>78</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C131">
         <v>2013</v>
@@ -3600,7 +3589,7 @@
         <v>78</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C132">
         <v>2013</v>
@@ -3620,7 +3609,7 @@
         <v>78</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C133">
         <v>2013</v>
@@ -3640,7 +3629,7 @@
         <v>78</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C134">
         <v>2013</v>
@@ -3660,7 +3649,7 @@
         <v>78</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C135">
         <v>2013</v>
@@ -3680,7 +3669,7 @@
         <v>78</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C136">
         <v>2013</v>
@@ -3700,7 +3689,7 @@
         <v>78</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C137">
         <v>2013</v>
@@ -3720,7 +3709,7 @@
         <v>78</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C138">
         <v>2013</v>
@@ -3740,7 +3729,7 @@
         <v>78</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>2013</v>
@@ -3760,7 +3749,7 @@
         <v>78</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C140">
         <v>2013</v>
@@ -3780,7 +3769,7 @@
         <v>78</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C141">
         <v>2013</v>
@@ -3800,7 +3789,7 @@
         <v>78</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C142">
         <v>2013</v>
@@ -3820,7 +3809,7 @@
         <v>78</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C143">
         <v>2013</v>
@@ -3840,7 +3829,7 @@
         <v>78</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C144">
         <v>2013</v>
@@ -3860,7 +3849,7 @@
         <v>78</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C145">
         <v>2013</v>
@@ -3880,7 +3869,7 @@
         <v>78</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C146">
         <v>2013</v>
@@ -3992,15 +3981,15 @@
         <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C152">
         <v>1981</v>
@@ -4012,15 +4001,15 @@
         <v>15</v>
       </c>
       <c r="F152" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C153">
         <v>1981</v>
@@ -4032,15 +4021,15 @@
         <v>14</v>
       </c>
       <c r="F153" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C154">
         <v>1981</v>
@@ -4052,15 +4041,15 @@
         <v>15</v>
       </c>
       <c r="F154" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C155">
         <v>1981</v>
@@ -4072,15 +4061,15 @@
         <v>15</v>
       </c>
       <c r="F155" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C156">
         <v>1981</v>
@@ -4092,15 +4081,15 @@
         <v>14</v>
       </c>
       <c r="F156" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C157">
         <v>1981</v>
@@ -4112,15 +4101,15 @@
         <v>14</v>
       </c>
       <c r="F157" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C158">
         <v>1985</v>
@@ -4137,10 +4126,10 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C159">
         <v>1985</v>
@@ -4152,15 +4141,15 @@
         <v>14</v>
       </c>
       <c r="F159" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C160">
         <v>1985</v>
@@ -4177,10 +4166,10 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C161">
         <v>1985</v>
@@ -4192,15 +4181,15 @@
         <v>15</v>
       </c>
       <c r="F161" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C162">
         <v>1985</v>
@@ -4217,10 +4206,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C163">
         <v>1985</v>
@@ -4232,15 +4221,15 @@
         <v>15</v>
       </c>
       <c r="F163" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C164">
         <v>1985</v>
@@ -4252,15 +4241,15 @@
         <v>14</v>
       </c>
       <c r="F164" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C165">
         <v>1985</v>
@@ -4277,10 +4266,10 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C166">
         <v>1985</v>
@@ -4297,10 +4286,10 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C167">
         <v>1985</v>
@@ -4317,10 +4306,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C168">
         <v>1988</v>
@@ -4332,15 +4321,15 @@
         <v>15</v>
       </c>
       <c r="F168" t="s">
-        <v>148</v>
+        <v>202</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C169">
         <v>1988</v>
@@ -4352,15 +4341,15 @@
         <v>14</v>
       </c>
       <c r="F169" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C170">
         <v>1988</v>
@@ -4377,10 +4366,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C171">
         <v>1988</v>
@@ -4392,15 +4381,15 @@
         <v>8</v>
       </c>
       <c r="F171" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C172">
         <v>1988</v>
@@ -4412,15 +4401,15 @@
         <v>14</v>
       </c>
       <c r="F172" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C173">
         <v>1988</v>
@@ -4437,10 +4426,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C174">
         <v>1990</v>
@@ -4457,10 +4446,10 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C175">
         <v>1990</v>
@@ -4472,15 +4461,15 @@
         <v>8</v>
       </c>
       <c r="F175" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C176">
         <v>1990</v>
@@ -4497,10 +4486,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C177">
         <v>1990</v>
@@ -4517,10 +4506,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C178">
         <v>1990</v>
@@ -4537,10 +4526,10 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C179">
         <v>1990</v>
@@ -4552,15 +4541,15 @@
         <v>15</v>
       </c>
       <c r="F179" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C180">
         <v>1990</v>
@@ -4572,15 +4561,15 @@
         <v>15</v>
       </c>
       <c r="F180" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C181">
         <v>1990</v>
@@ -4592,15 +4581,15 @@
         <v>8</v>
       </c>
       <c r="F181" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C182">
         <v>1990</v>
@@ -4612,15 +4601,15 @@
         <v>14</v>
       </c>
       <c r="F182" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C183">
         <v>1990</v>
@@ -4632,15 +4621,15 @@
         <v>15</v>
       </c>
       <c r="F183" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C184">
         <v>1990</v>
@@ -4657,10 +4646,10 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C185">
         <v>1990</v>
@@ -4672,15 +4661,15 @@
         <v>15</v>
       </c>
       <c r="F185" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C186">
         <v>1990</v>
@@ -4697,10 +4686,10 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C187">
         <v>1990</v>
@@ -4712,15 +4701,15 @@
         <v>15</v>
       </c>
       <c r="F187" t="s">
-        <v>154</v>
+        <v>203</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C188">
         <v>1990</v>
@@ -4732,15 +4721,15 @@
         <v>14</v>
       </c>
       <c r="F188" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C189">
         <v>1991</v>
@@ -4757,10 +4746,10 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C190">
         <v>1991</v>
@@ -4777,10 +4766,10 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C191">
         <v>1991</v>
@@ -4797,10 +4786,10 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C192">
         <v>1991</v>
@@ -4812,15 +4801,15 @@
         <v>15</v>
       </c>
       <c r="F192" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C193">
         <v>1991</v>
@@ -4837,10 +4826,10 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C194">
         <v>1991</v>
@@ -4852,15 +4841,15 @@
         <v>15</v>
       </c>
       <c r="F194" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C195">
         <v>1991</v>
@@ -4877,10 +4866,10 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C196">
         <v>1991</v>
@@ -4892,15 +4881,15 @@
         <v>15</v>
       </c>
       <c r="F196" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C197">
         <v>1991</v>
@@ -4912,15 +4901,15 @@
         <v>15</v>
       </c>
       <c r="F197" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C198">
         <v>1994</v>
@@ -4937,10 +4926,10 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C199">
         <v>1994</v>
@@ -4952,15 +4941,15 @@
         <v>8</v>
       </c>
       <c r="F199" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C200">
         <v>1994</v>
@@ -4972,15 +4961,15 @@
         <v>15</v>
       </c>
       <c r="F200" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C201">
         <v>1994</v>
@@ -4992,35 +4981,35 @@
         <v>15</v>
       </c>
       <c r="F201" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C202">
         <v>1994</v>
       </c>
       <c r="D202" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E202" t="s">
         <v>15</v>
       </c>
       <c r="F202" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C203">
         <v>1994</v>
@@ -5037,10 +5026,10 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C204">
         <v>1994</v>
@@ -5057,10 +5046,10 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C205">
         <v>1994</v>
@@ -5077,10 +5066,10 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C206">
         <v>1994</v>
@@ -5097,10 +5086,10 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C207">
         <v>1994</v>
@@ -5112,21 +5101,21 @@
         <v>14</v>
       </c>
       <c r="F207" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C208">
         <v>1994</v>
       </c>
       <c r="D208" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E208" t="s">
         <v>14</v>
@@ -5137,10 +5126,10 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C209">
         <v>1995</v>
@@ -5157,10 +5146,10 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C210">
         <v>1995</v>
@@ -5172,15 +5161,15 @@
         <v>14</v>
       </c>
       <c r="F210" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C211">
         <v>1995</v>
@@ -5197,10 +5186,10 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C212">
         <v>1995</v>
@@ -5217,10 +5206,10 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C213">
         <v>1995</v>
@@ -5237,10 +5226,10 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C214">
         <v>1995</v>
@@ -5257,10 +5246,10 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C215">
         <v>1995</v>
@@ -5277,10 +5266,10 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C216">
         <v>1995</v>
@@ -5292,15 +5281,15 @@
         <v>8</v>
       </c>
       <c r="F216" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C217">
         <v>1995</v>
@@ -5312,15 +5301,15 @@
         <v>8</v>
       </c>
       <c r="F217" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C218">
         <v>1995</v>
@@ -5337,10 +5326,10 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C219">
         <v>1995</v>
@@ -5357,10 +5346,10 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C220">
         <v>1996</v>
@@ -5377,10 +5366,10 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C221">
         <v>1996</v>
@@ -5392,15 +5381,15 @@
         <v>14</v>
       </c>
       <c r="F221" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C222">
         <v>1996</v>
@@ -5412,15 +5401,15 @@
         <v>8</v>
       </c>
       <c r="F222" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C223">
         <v>1996</v>
@@ -5432,15 +5421,15 @@
         <v>14</v>
       </c>
       <c r="F223" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C224">
         <v>1996</v>
@@ -5452,15 +5441,15 @@
         <v>14</v>
       </c>
       <c r="F224" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C225">
         <v>1996</v>
@@ -5472,15 +5461,15 @@
         <v>14</v>
       </c>
       <c r="F225" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C226">
         <v>1996</v>
@@ -5492,15 +5481,15 @@
         <v>14</v>
       </c>
       <c r="F226" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C227">
         <v>1996</v>
@@ -5512,15 +5501,15 @@
         <v>14</v>
       </c>
       <c r="F227" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C228">
         <v>1996</v>
@@ -5537,10 +5526,10 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C229">
         <v>1996</v>
@@ -5552,15 +5541,15 @@
         <v>14</v>
       </c>
       <c r="F229" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C230">
         <v>1996</v>
@@ -5572,15 +5561,15 @@
         <v>14</v>
       </c>
       <c r="F230" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C231">
         <v>1996</v>
@@ -5592,15 +5581,15 @@
         <v>14</v>
       </c>
       <c r="F231" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C232">
         <v>1996</v>
@@ -5612,15 +5601,15 @@
         <v>8</v>
       </c>
       <c r="F232" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C233">
         <v>1996</v>
@@ -5637,36 +5626,36 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C234">
         <v>1996</v>
       </c>
       <c r="D234" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E234" t="s">
         <v>8</v>
       </c>
       <c r="F234" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C235">
         <v>1996</v>
       </c>
       <c r="D235" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E235" t="s">
         <v>8</v>
@@ -5677,16 +5666,16 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C236">
         <v>1996</v>
       </c>
       <c r="D236" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E236" t="s">
         <v>8</v>
@@ -5697,16 +5686,16 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C237">
         <v>1996</v>
       </c>
       <c r="D237" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E237" t="s">
         <v>14</v>
@@ -5717,16 +5706,16 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C238">
         <v>1996</v>
       </c>
       <c r="D238" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E238" t="s">
         <v>8</v>
@@ -5737,70 +5726,70 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C239">
         <v>1996</v>
       </c>
       <c r="D239" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E239" t="s">
         <v>8</v>
       </c>
       <c r="F239" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C240">
         <v>1996</v>
       </c>
       <c r="D240" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E240" t="s">
         <v>8</v>
       </c>
       <c r="F240" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C241">
         <v>1996</v>
       </c>
       <c r="D241" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E241" t="s">
         <v>8</v>
       </c>
       <c r="F241" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C242">
         <v>1997</v>
@@ -5817,10 +5806,10 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C243">
         <v>1997</v>
@@ -5837,10 +5826,10 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C244">
         <v>1997</v>
@@ -5852,15 +5841,15 @@
         <v>15</v>
       </c>
       <c r="F244" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C245">
         <v>1997</v>
@@ -5872,15 +5861,15 @@
         <v>15</v>
       </c>
       <c r="F245" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C246">
         <v>1997</v>
@@ -5897,10 +5886,10 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C247">
         <v>1997</v>
@@ -5917,10 +5906,10 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C248">
         <v>1997</v>
@@ -5932,15 +5921,15 @@
         <v>14</v>
       </c>
       <c r="F248" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C249">
         <v>1998</v>
@@ -5957,10 +5946,10 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C250">
         <v>1998</v>
@@ -5972,15 +5961,15 @@
         <v>14</v>
       </c>
       <c r="F250" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C251">
         <v>1998</v>
@@ -5997,56 +5986,56 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C252">
         <v>1998</v>
       </c>
       <c r="D252" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E252" t="s">
         <v>15</v>
       </c>
       <c r="F252" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C253">
         <v>1998</v>
       </c>
       <c r="D253" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E253" t="s">
         <v>14</v>
       </c>
       <c r="F253" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C254">
         <v>1998</v>
       </c>
       <c r="D254" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E254" t="s">
         <v>15</v>
@@ -6057,10 +6046,10 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C255">
         <v>1998</v>
@@ -6077,10 +6066,10 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C256">
         <v>1998</v>
@@ -6097,10 +6086,10 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C257">
         <v>2000</v>
@@ -6117,10 +6106,10 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C258">
         <v>2000</v>
@@ -6132,15 +6121,15 @@
         <v>14</v>
       </c>
       <c r="F258" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C259">
         <v>2000</v>
@@ -6157,10 +6146,10 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C260">
         <v>2000</v>

</xml_diff>

<commit_message>
ADD LABELING FOR MAIN INTEREST GROUP
</commit_message>
<xml_diff>
--- a/Interest-group-09-25.xlsx
+++ b/Interest-group-09-25.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haowang/Documents/Amicus-Brief/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Amicus-Brief\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="19740" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="576" yWindow="456" windowWidth="19740" windowHeight="14676" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Interest-group-09-15" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="204">
   <si>
     <t>CASE-NAME</t>
   </si>
@@ -633,12 +633,15 @@
   </si>
   <si>
     <t>NATIONAL BLACK MEDIA COALITION</t>
+  </si>
+  <si>
+    <t>MAJOR-INVOLVED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -680,6 +683,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -948,20 +954,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F260"/>
+  <dimension ref="A1:H260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="F248" sqref="F248"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H260" sqref="H260"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="57.6640625" customWidth="1"/>
-    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1"/>
+    <col min="4" max="4" width="57.69921875" customWidth="1"/>
+    <col min="6" max="6" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,8 +986,11 @@
       <c r="F1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1000,8 +1009,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1020,8 +1032,11 @@
       <c r="F3" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1040,8 +1055,11 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1060,8 +1078,11 @@
       <c r="F5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1080,8 +1101,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1100,8 +1124,11 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1120,8 +1147,11 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1140,8 +1170,11 @@
       <c r="F9" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1160,8 +1193,11 @@
       <c r="F10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1180,8 +1216,11 @@
       <c r="F11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1200,8 +1239,11 @@
       <c r="F12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1220,8 +1262,11 @@
       <c r="F13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1240,8 +1285,11 @@
       <c r="F14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1260,8 +1308,11 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1280,8 +1331,11 @@
       <c r="F16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1300,8 +1354,11 @@
       <c r="F17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1320,8 +1377,11 @@
       <c r="F18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1340,8 +1400,11 @@
       <c r="F19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -1360,8 +1423,11 @@
       <c r="F20" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -1380,8 +1446,11 @@
       <c r="F21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>113</v>
       </c>
@@ -1400,8 +1469,11 @@
       <c r="F22" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -1420,8 +1492,11 @@
       <c r="F23" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -1440,8 +1515,11 @@
       <c r="F24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>113</v>
       </c>
@@ -1460,8 +1538,11 @@
       <c r="F25" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -1480,8 +1561,11 @@
       <c r="F26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -1500,8 +1584,11 @@
       <c r="F27" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -1520,8 +1607,11 @@
       <c r="F28" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -1540,8 +1630,11 @@
       <c r="F29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -1560,8 +1653,11 @@
       <c r="F30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -1580,8 +1676,11 @@
       <c r="F31" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -1600,8 +1699,11 @@
       <c r="F32" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1620,8 +1722,11 @@
       <c r="F33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1640,8 +1745,11 @@
       <c r="F34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1660,8 +1768,11 @@
       <c r="F35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1680,8 +1791,11 @@
       <c r="F36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1700,8 +1814,11 @@
       <c r="F37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1720,8 +1837,11 @@
       <c r="F38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1740,8 +1860,11 @@
       <c r="F39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1760,8 +1883,11 @@
       <c r="F40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1780,8 +1906,11 @@
       <c r="F41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -1800,8 +1929,11 @@
       <c r="F42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1820,8 +1952,11 @@
       <c r="F43" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1840,8 +1975,11 @@
       <c r="F44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1860,8 +1998,11 @@
       <c r="F45" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1880,8 +2021,11 @@
       <c r="F46" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1900,8 +2044,11 @@
       <c r="F47" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1920,8 +2067,11 @@
       <c r="F48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1940,8 +2090,11 @@
       <c r="F49" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1952,16 +2105,19 @@
         <v>2009</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -1980,8 +2136,11 @@
       <c r="F51" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -2000,8 +2159,11 @@
       <c r="F52" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>119</v>
       </c>
@@ -2020,8 +2182,11 @@
       <c r="F53" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -2040,8 +2205,11 @@
       <c r="F54" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -2060,8 +2228,11 @@
       <c r="F55" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -2080,8 +2251,11 @@
       <c r="F56" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>119</v>
       </c>
@@ -2100,8 +2274,11 @@
       <c r="F57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -2120,8 +2297,11 @@
       <c r="F58" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -2140,8 +2320,11 @@
       <c r="F59" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -2160,8 +2343,11 @@
       <c r="F60" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -2180,8 +2366,11 @@
       <c r="F61" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -2200,8 +2389,11 @@
       <c r="F62" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -2220,8 +2412,11 @@
       <c r="F63" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>119</v>
       </c>
@@ -2240,8 +2435,11 @@
       <c r="F64" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -2260,8 +2458,11 @@
       <c r="F65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -2280,8 +2481,11 @@
       <c r="F66" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>119</v>
       </c>
@@ -2300,8 +2504,11 @@
       <c r="F67" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -2320,8 +2527,11 @@
       <c r="F68" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>119</v>
       </c>
@@ -2340,8 +2550,11 @@
       <c r="F69" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -2360,8 +2573,11 @@
       <c r="F70" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>119</v>
       </c>
@@ -2380,8 +2596,11 @@
       <c r="F71" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -2400,8 +2619,11 @@
       <c r="F72" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -2420,8 +2642,11 @@
       <c r="F73" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -2440,8 +2665,11 @@
       <c r="F74" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2460,8 +2688,11 @@
       <c r="F75" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2480,8 +2711,11 @@
       <c r="F76" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2500,8 +2734,11 @@
       <c r="F77" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -2520,8 +2757,11 @@
       <c r="F78" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2540,8 +2780,11 @@
       <c r="F79" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>52</v>
       </c>
@@ -2560,8 +2803,11 @@
       <c r="F80" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>52</v>
       </c>
@@ -2580,8 +2826,11 @@
       <c r="F81" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -2600,8 +2849,11 @@
       <c r="F82" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>52</v>
       </c>
@@ -2620,8 +2872,11 @@
       <c r="F83" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>52</v>
       </c>
@@ -2640,8 +2895,11 @@
       <c r="F84" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>52</v>
       </c>
@@ -2660,8 +2918,11 @@
       <c r="F85" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>52</v>
       </c>
@@ -2680,8 +2941,11 @@
       <c r="F86" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>52</v>
       </c>
@@ -2700,8 +2964,11 @@
       <c r="F87" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>52</v>
       </c>
@@ -2720,8 +2987,11 @@
       <c r="F88" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>52</v>
       </c>
@@ -2740,8 +3010,11 @@
       <c r="F89" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>52</v>
       </c>
@@ -2760,8 +3033,11 @@
       <c r="F90" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>52</v>
       </c>
@@ -2780,8 +3056,11 @@
       <c r="F91" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>52</v>
       </c>
@@ -2800,8 +3079,11 @@
       <c r="F92" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>52</v>
       </c>
@@ -2820,8 +3102,11 @@
       <c r="F93" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>52</v>
       </c>
@@ -2840,8 +3125,11 @@
       <c r="F94" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>52</v>
       </c>
@@ -2860,8 +3148,11 @@
       <c r="F95" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>52</v>
       </c>
@@ -2880,8 +3171,11 @@
       <c r="F96" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>52</v>
       </c>
@@ -2900,8 +3194,11 @@
       <c r="F97" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>52</v>
       </c>
@@ -2920,8 +3217,11 @@
       <c r="F98" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>52</v>
       </c>
@@ -2940,8 +3240,11 @@
       <c r="F99" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>52</v>
       </c>
@@ -2960,8 +3263,11 @@
       <c r="F100" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -2980,8 +3286,11 @@
       <c r="F101" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>52</v>
       </c>
@@ -3000,8 +3309,11 @@
       <c r="F102" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -3020,8 +3332,11 @@
       <c r="F103" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -3040,8 +3355,11 @@
       <c r="F104" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -3060,8 +3378,11 @@
       <c r="F105" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>78</v>
       </c>
@@ -3080,8 +3401,11 @@
       <c r="F106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>78</v>
       </c>
@@ -3100,8 +3424,11 @@
       <c r="F107" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>78</v>
       </c>
@@ -3120,8 +3447,11 @@
       <c r="F108" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>78</v>
       </c>
@@ -3140,8 +3470,11 @@
       <c r="F109" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>78</v>
       </c>
@@ -3160,8 +3493,11 @@
       <c r="F110" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>78</v>
       </c>
@@ -3180,8 +3516,11 @@
       <c r="F111" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>78</v>
       </c>
@@ -3200,8 +3539,11 @@
       <c r="F112" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>78</v>
       </c>
@@ -3220,8 +3562,11 @@
       <c r="F113" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>78</v>
       </c>
@@ -3240,8 +3585,11 @@
       <c r="F114" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>78</v>
       </c>
@@ -3260,8 +3608,11 @@
       <c r="F115" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>78</v>
       </c>
@@ -3280,8 +3631,11 @@
       <c r="F116" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>78</v>
       </c>
@@ -3300,8 +3654,11 @@
       <c r="F117" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>78</v>
       </c>
@@ -3320,8 +3677,11 @@
       <c r="F118" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>78</v>
       </c>
@@ -3340,8 +3700,11 @@
       <c r="F119" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>78</v>
       </c>
@@ -3360,8 +3723,11 @@
       <c r="F120" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>78</v>
       </c>
@@ -3380,8 +3746,11 @@
       <c r="F121" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>78</v>
       </c>
@@ -3400,8 +3769,11 @@
       <c r="F122" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>78</v>
       </c>
@@ -3420,8 +3792,11 @@
       <c r="F123" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>78</v>
       </c>
@@ -3440,8 +3815,11 @@
       <c r="F124" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>78</v>
       </c>
@@ -3460,8 +3838,11 @@
       <c r="F125" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>78</v>
       </c>
@@ -3480,8 +3861,11 @@
       <c r="F126" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>78</v>
       </c>
@@ -3500,8 +3884,11 @@
       <c r="F127" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>78</v>
       </c>
@@ -3520,8 +3907,11 @@
       <c r="F128" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>78</v>
       </c>
@@ -3540,8 +3930,11 @@
       <c r="F129" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>78</v>
       </c>
@@ -3560,8 +3953,11 @@
       <c r="F130" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>78</v>
       </c>
@@ -3580,8 +3976,11 @@
       <c r="F131" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>78</v>
       </c>
@@ -3600,8 +3999,11 @@
       <c r="F132" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>78</v>
       </c>
@@ -3620,8 +4022,11 @@
       <c r="F133" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>78</v>
       </c>
@@ -3640,8 +4045,11 @@
       <c r="F134" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>78</v>
       </c>
@@ -3660,8 +4068,11 @@
       <c r="F135" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>78</v>
       </c>
@@ -3680,8 +4091,11 @@
       <c r="F136" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>78</v>
       </c>
@@ -3700,8 +4114,11 @@
       <c r="F137" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>78</v>
       </c>
@@ -3720,8 +4137,11 @@
       <c r="F138" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>78</v>
       </c>
@@ -3740,8 +4160,11 @@
       <c r="F139" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>78</v>
       </c>
@@ -3760,8 +4183,11 @@
       <c r="F140" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>78</v>
       </c>
@@ -3780,8 +4206,11 @@
       <c r="F141" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>78</v>
       </c>
@@ -3800,8 +4229,11 @@
       <c r="F142" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>78</v>
       </c>
@@ -3820,8 +4252,11 @@
       <c r="F143" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>78</v>
       </c>
@@ -3840,8 +4275,11 @@
       <c r="F144" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>78</v>
       </c>
@@ -3860,8 +4298,11 @@
       <c r="F145" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>78</v>
       </c>
@@ -3880,8 +4321,11 @@
       <c r="F146" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>110</v>
       </c>
@@ -3900,8 +4344,11 @@
       <c r="F147" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>110</v>
       </c>
@@ -3920,8 +4367,11 @@
       <c r="F148" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>110</v>
       </c>
@@ -3940,8 +4390,11 @@
       <c r="F149" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>110</v>
       </c>
@@ -3960,8 +4413,11 @@
       <c r="F150" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>110</v>
       </c>
@@ -3980,8 +4436,11 @@
       <c r="F151" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>129</v>
       </c>
@@ -4000,8 +4459,11 @@
       <c r="F152" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -4020,8 +4482,11 @@
       <c r="F153" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>129</v>
       </c>
@@ -4040,8 +4505,11 @@
       <c r="F154" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>129</v>
       </c>
@@ -4060,8 +4528,11 @@
       <c r="F155" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>129</v>
       </c>
@@ -4080,8 +4551,11 @@
       <c r="F156" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>129</v>
       </c>
@@ -4100,8 +4574,11 @@
       <c r="F157" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>162</v>
       </c>
@@ -4120,8 +4597,11 @@
       <c r="F158" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>162</v>
       </c>
@@ -4140,8 +4620,11 @@
       <c r="F159" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>135</v>
       </c>
@@ -4160,8 +4643,11 @@
       <c r="F160" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>135</v>
       </c>
@@ -4180,8 +4666,11 @@
       <c r="F161" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>135</v>
       </c>
@@ -4200,8 +4689,11 @@
       <c r="F162" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>135</v>
       </c>
@@ -4220,8 +4712,11 @@
       <c r="F163" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>135</v>
       </c>
@@ -4240,8 +4735,11 @@
       <c r="F164" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>135</v>
       </c>
@@ -4260,8 +4758,11 @@
       <c r="F165" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>135</v>
       </c>
@@ -4280,8 +4781,11 @@
       <c r="F166" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>135</v>
       </c>
@@ -4300,8 +4804,11 @@
       <c r="F167" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>138</v>
       </c>
@@ -4320,8 +4827,11 @@
       <c r="F168" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>138</v>
       </c>
@@ -4340,8 +4850,11 @@
       <c r="F169" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>138</v>
       </c>
@@ -4360,8 +4873,11 @@
       <c r="F170" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>138</v>
       </c>
@@ -4380,8 +4896,11 @@
       <c r="F171" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>138</v>
       </c>
@@ -4400,8 +4919,11 @@
       <c r="F172" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>138</v>
       </c>
@@ -4420,8 +4942,11 @@
       <c r="F173" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>163</v>
       </c>
@@ -4440,8 +4965,11 @@
       <c r="F174" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>163</v>
       </c>
@@ -4460,8 +4988,11 @@
       <c r="F175" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>163</v>
       </c>
@@ -4480,8 +5011,11 @@
       <c r="F176" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>163</v>
       </c>
@@ -4500,8 +5034,11 @@
       <c r="F177" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>164</v>
       </c>
@@ -4520,8 +5057,11 @@
       <c r="F178" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>164</v>
       </c>
@@ -4540,8 +5080,11 @@
       <c r="F179" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>164</v>
       </c>
@@ -4560,8 +5103,11 @@
       <c r="F180" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>164</v>
       </c>
@@ -4580,8 +5126,11 @@
       <c r="F181" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>164</v>
       </c>
@@ -4600,8 +5149,11 @@
       <c r="F182" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>164</v>
       </c>
@@ -4620,8 +5172,11 @@
       <c r="F183" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>142</v>
       </c>
@@ -4640,8 +5195,11 @@
       <c r="F184" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>142</v>
       </c>
@@ -4660,8 +5218,11 @@
       <c r="F185" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>142</v>
       </c>
@@ -4680,8 +5241,11 @@
       <c r="F186" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>142</v>
       </c>
@@ -4700,8 +5264,11 @@
       <c r="F187" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>142</v>
       </c>
@@ -4720,8 +5287,11 @@
       <c r="F188" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>168</v>
       </c>
@@ -4740,8 +5310,11 @@
       <c r="F189" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>168</v>
       </c>
@@ -4760,8 +5333,11 @@
       <c r="F190" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>168</v>
       </c>
@@ -4780,8 +5356,11 @@
       <c r="F191" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>168</v>
       </c>
@@ -4800,8 +5379,11 @@
       <c r="F192" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>168</v>
       </c>
@@ -4820,8 +5402,11 @@
       <c r="F193" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>168</v>
       </c>
@@ -4840,8 +5425,11 @@
       <c r="F194" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>168</v>
       </c>
@@ -4860,8 +5448,11 @@
       <c r="F195" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>168</v>
       </c>
@@ -4880,8 +5471,11 @@
       <c r="F196" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>168</v>
       </c>
@@ -4900,8 +5494,11 @@
       <c r="F197" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>171</v>
       </c>
@@ -4920,8 +5517,11 @@
       <c r="F198" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>171</v>
       </c>
@@ -4940,8 +5540,11 @@
       <c r="F199" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>171</v>
       </c>
@@ -4960,8 +5563,11 @@
       <c r="F200" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>171</v>
       </c>
@@ -4980,8 +5586,11 @@
       <c r="F201" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>171</v>
       </c>
@@ -5000,8 +5609,11 @@
       <c r="F202" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>171</v>
       </c>
@@ -5020,8 +5632,11 @@
       <c r="F203" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>171</v>
       </c>
@@ -5040,8 +5655,11 @@
       <c r="F204" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>171</v>
       </c>
@@ -5060,8 +5678,11 @@
       <c r="F205" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>171</v>
       </c>
@@ -5080,8 +5701,11 @@
       <c r="F206" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>171</v>
       </c>
@@ -5100,8 +5724,11 @@
       <c r="F207" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>171</v>
       </c>
@@ -5120,8 +5747,11 @@
       <c r="F208" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>145</v>
       </c>
@@ -5140,8 +5770,11 @@
       <c r="F209" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>145</v>
       </c>
@@ -5160,8 +5793,11 @@
       <c r="F210" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>145</v>
       </c>
@@ -5180,8 +5816,11 @@
       <c r="F211" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>145</v>
       </c>
@@ -5200,8 +5839,11 @@
       <c r="F212" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>145</v>
       </c>
@@ -5220,8 +5862,11 @@
       <c r="F213" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>145</v>
       </c>
@@ -5240,8 +5885,11 @@
       <c r="F214" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>145</v>
       </c>
@@ -5260,8 +5908,11 @@
       <c r="F215" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>145</v>
       </c>
@@ -5280,8 +5931,11 @@
       <c r="F216" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>145</v>
       </c>
@@ -5300,8 +5954,11 @@
       <c r="F217" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>145</v>
       </c>
@@ -5320,8 +5977,11 @@
       <c r="F218" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>145</v>
       </c>
@@ -5340,8 +6000,11 @@
       <c r="F219" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>177</v>
       </c>
@@ -5360,8 +6023,11 @@
       <c r="F220" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>177</v>
       </c>
@@ -5380,8 +6046,11 @@
       <c r="F221" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>177</v>
       </c>
@@ -5400,8 +6069,11 @@
       <c r="F222" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>177</v>
       </c>
@@ -5420,8 +6092,11 @@
       <c r="F223" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>177</v>
       </c>
@@ -5440,8 +6115,11 @@
       <c r="F224" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>177</v>
       </c>
@@ -5460,8 +6138,11 @@
       <c r="F225" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>177</v>
       </c>
@@ -5480,8 +6161,11 @@
       <c r="F226" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>177</v>
       </c>
@@ -5500,8 +6184,11 @@
       <c r="F227" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>177</v>
       </c>
@@ -5520,8 +6207,11 @@
       <c r="F228" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>177</v>
       </c>
@@ -5540,8 +6230,11 @@
       <c r="F229" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>177</v>
       </c>
@@ -5560,8 +6253,11 @@
       <c r="F230" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>177</v>
       </c>
@@ -5580,8 +6276,11 @@
       <c r="F231" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>177</v>
       </c>
@@ -5600,8 +6299,11 @@
       <c r="F232" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>177</v>
       </c>
@@ -5620,8 +6322,11 @@
       <c r="F233" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>177</v>
       </c>
@@ -5640,8 +6345,11 @@
       <c r="F234" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>177</v>
       </c>
@@ -5660,8 +6368,11 @@
       <c r="F235" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>177</v>
       </c>
@@ -5680,8 +6391,11 @@
       <c r="F236" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>177</v>
       </c>
@@ -5700,8 +6414,11 @@
       <c r="F237" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>177</v>
       </c>
@@ -5720,8 +6437,11 @@
       <c r="F238" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>177</v>
       </c>
@@ -5740,8 +6460,11 @@
       <c r="F239" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>177</v>
       </c>
@@ -5760,8 +6483,11 @@
       <c r="F240" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>177</v>
       </c>
@@ -5780,8 +6506,11 @@
       <c r="F241" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>190</v>
       </c>
@@ -5800,8 +6529,11 @@
       <c r="F242" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>190</v>
       </c>
@@ -5820,8 +6552,11 @@
       <c r="F243" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>190</v>
       </c>
@@ -5840,8 +6575,11 @@
       <c r="F244" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>190</v>
       </c>
@@ -5860,8 +6598,11 @@
       <c r="F245" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>190</v>
       </c>
@@ -5880,8 +6621,11 @@
       <c r="F246" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>190</v>
       </c>
@@ -5900,8 +6644,11 @@
       <c r="F247" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>190</v>
       </c>
@@ -5920,8 +6667,11 @@
       <c r="F248" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>147</v>
       </c>
@@ -5940,8 +6690,11 @@
       <c r="F249" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>147</v>
       </c>
@@ -5960,8 +6713,11 @@
       <c r="F250" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>147</v>
       </c>
@@ -5980,8 +6736,11 @@
       <c r="F251" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>147</v>
       </c>
@@ -6000,8 +6759,11 @@
       <c r="F252" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>147</v>
       </c>
@@ -6020,8 +6782,11 @@
       <c r="F253" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>147</v>
       </c>
@@ -6040,8 +6805,11 @@
       <c r="F254" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>193</v>
       </c>
@@ -6060,8 +6828,11 @@
       <c r="F255" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>193</v>
       </c>
@@ -6080,8 +6851,11 @@
       <c r="F256" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>194</v>
       </c>
@@ -6100,8 +6874,11 @@
       <c r="F257" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>194</v>
       </c>
@@ -6120,8 +6897,11 @@
       <c r="F258" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>194</v>
       </c>
@@ -6140,8 +6920,11 @@
       <c r="F259" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>194</v>
       </c>
@@ -6159,6 +6942,9 @@
       </c>
       <c r="F260" t="s">
         <v>9</v>
+      </c>
+      <c r="H260">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>